<commit_message>
Added LogInPage Test Cases
</commit_message>
<xml_diff>
--- a/TestData/Excel_Files/LoginCredentialDetails.xlsx
+++ b/TestData/Excel_Files/LoginCredentialDetails.xlsx
@@ -1,18 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{46E396AC-0034-403E-9B14-417331178756}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AWT Tester\eclipse-workspace\Awt_Project_Managment\TestData\Excel_Files\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B35EFB9-5F19-4619-B13F-6B22054DE10D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{E28CADD0-9E9C-48D6-9692-C4E6C50E8CDC}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{E28CADD0-9E9C-48D6-9692-C4E6C50E8CDC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="verifyLogInCredentialsTest" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:C16"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="19">
   <si>
     <t>TestCaseId</t>
   </si>
@@ -54,7 +58,31 @@
     <t>OperatorScada#@2023</t>
   </si>
   <si>
-    <t>abcd</t>
+    <t>APMS-T132</t>
+  </si>
+  <si>
+    <t>APMS-T133</t>
+  </si>
+  <si>
+    <t>APMS-T134</t>
+  </si>
+  <si>
+    <t>APMS-T135</t>
+  </si>
+  <si>
+    <t>Tesla</t>
+  </si>
+  <si>
+    <t>APMS-T136</t>
+  </si>
+  <si>
+    <t>Tesla@123</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Testing@123</t>
   </si>
 </sst>
 </file>
@@ -111,7 +139,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -122,6 +150,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -457,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8C46E38-2B1E-4402-BDC5-292DA50A6E9F}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -493,8 +522,8 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="1">
-        <v>290</v>
+      <c r="A3" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>6</v>
@@ -504,8 +533,8 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="1">
-        <v>290</v>
+      <c r="A4" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>8</v>
@@ -515,14 +544,32 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="1">
-        <v>290</v>
+      <c r="A5" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>9</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="4"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -531,6 +578,7 @@
     <hyperlink ref="C3" r:id="rId1" xr:uid="{4F447B3B-61D5-4B84-98CA-BB2FB17AF9C6}"/>
     <hyperlink ref="C4" r:id="rId2" xr:uid="{44FA3455-F433-4672-8747-96EBABF495F1}"/>
     <hyperlink ref="C5" r:id="rId3" xr:uid="{F70F74DB-E0ED-497D-A46A-A80DE8B48C29}"/>
+    <hyperlink ref="C7" r:id="rId4" xr:uid="{C0621982-136A-40A3-8716-B92ED6211AB7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -540,8 +588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{131E6503-DC84-4BD8-8FD2-EF0D8A7E2F03}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
add forgot panel test cases and wrote Gmail APi Code for taking otp from gmail
</commit_message>
<xml_diff>
--- a/TestData/Excel_Files/LoginCredentialDetails.xlsx
+++ b/TestData/Excel_Files/LoginCredentialDetails.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AWT Tester\eclipse-workspace\Awt_Project_Managment\TestData\Excel_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B35EFB9-5F19-4619-B13F-6B22054DE10D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ED44920-ECA1-4AF4-805C-A1E656F6FB2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{E28CADD0-9E9C-48D6-9692-C4E6C50E8CDC}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
   <si>
     <t>TestCaseId</t>
   </si>
@@ -83,6 +83,21 @@
   </si>
   <si>
     <t>Testing@123</t>
+  </si>
+  <si>
+    <t>APMS-T143</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>awtindia.sc@gmail.com</t>
+  </si>
+  <si>
+    <t>APMS-T144</t>
+  </si>
+  <si>
+    <t>nicoalastestla458@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -486,10 +501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8C46E38-2B1E-4402-BDC5-292DA50A6E9F}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -497,9 +512,10 @@
     <col min="1" max="1" width="30.81640625" customWidth="1"/>
     <col min="2" max="2" width="27.453125" customWidth="1"/>
     <col min="3" max="3" width="28.26953125" customWidth="1"/>
+    <col min="4" max="4" width="28.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -509,8 +525,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -521,7 +540,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -532,7 +551,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -543,7 +562,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -554,7 +573,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -563,13 +582,29 @@
       </c>
       <c r="C6" s="4"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="4" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -579,6 +614,7 @@
     <hyperlink ref="C4" r:id="rId2" xr:uid="{44FA3455-F433-4672-8747-96EBABF495F1}"/>
     <hyperlink ref="C5" r:id="rId3" xr:uid="{F70F74DB-E0ED-497D-A46A-A80DE8B48C29}"/>
     <hyperlink ref="C7" r:id="rId4" xr:uid="{C0621982-136A-40A3-8716-B92ED6211AB7}"/>
+    <hyperlink ref="D9" r:id="rId5" xr:uid="{4E0708DC-BCB8-48B2-93AB-7B6268B178F0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added all Forgot and Reset Password Test Cases and add new Login xl file
</commit_message>
<xml_diff>
--- a/TestData/Excel_Files/LoginCredentialDetails.xlsx
+++ b/TestData/Excel_Files/LoginCredentialDetails.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AWT Tester\eclipse-workspace\Awt_Project_Managment\TestData\Excel_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ED44920-ECA1-4AF4-805C-A1E656F6FB2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04010B0B-C1DD-4831-8438-36C73F0E56F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{E28CADD0-9E9C-48D6-9692-C4E6C50E8CDC}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
   <si>
     <t>TestCaseId</t>
   </si>
@@ -98,6 +98,24 @@
   </si>
   <si>
     <t>nicoalastestla458@gmail.com</t>
+  </si>
+  <si>
+    <t>APMS-T153</t>
+  </si>
+  <si>
+    <t>Ankit@123</t>
+  </si>
+  <si>
+    <t>APMS-T154</t>
+  </si>
+  <si>
+    <t>AnkitYadav@1234</t>
+  </si>
+  <si>
+    <t>APMS-T155</t>
+  </si>
+  <si>
+    <t>AnkitYadav@12345$</t>
   </si>
 </sst>
 </file>
@@ -501,10 +519,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8C46E38-2B1E-4402-BDC5-292DA50A6E9F}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -607,6 +625,30 @@
         <v>23</v>
       </c>
     </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -615,6 +657,9 @@
     <hyperlink ref="C5" r:id="rId3" xr:uid="{F70F74DB-E0ED-497D-A46A-A80DE8B48C29}"/>
     <hyperlink ref="C7" r:id="rId4" xr:uid="{C0621982-136A-40A3-8716-B92ED6211AB7}"/>
     <hyperlink ref="D9" r:id="rId5" xr:uid="{4E0708DC-BCB8-48B2-93AB-7B6268B178F0}"/>
+    <hyperlink ref="C10" r:id="rId6" xr:uid="{37D55B64-07BD-4510-9561-D5D4C639590C}"/>
+    <hyperlink ref="C11" r:id="rId7" xr:uid="{D988B4E8-12C5-482E-8303-D3DA0A78FBB9}"/>
+    <hyperlink ref="C12" r:id="rId8" xr:uid="{F434B21B-56F0-47FD-8CFC-7C51B5862AE5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Completed LoginPage Test Cases
</commit_message>
<xml_diff>
--- a/TestData/Excel_Files/LoginCredentialDetails.xlsx
+++ b/TestData/Excel_Files/LoginCredentialDetails.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AWT Tester\eclipse-workspace\Awt_Project_Managment\TestData\Excel_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04010B0B-C1DD-4831-8438-36C73F0E56F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{955B28A6-D69B-45ED-AFE4-32C908FF5FA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{E28CADD0-9E9C-48D6-9692-C4E6C50E8CDC}"/>
+    <workbookView xWindow="2580" yWindow="2580" windowWidth="14400" windowHeight="7270" xr2:uid="{E28CADD0-9E9C-48D6-9692-C4E6C50E8CDC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -521,8 +521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8C46E38-2B1E-4402-BDC5-292DA50A6E9F}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
changes done in loginPage Test and added irrigation module  under that all the module and clasess
</commit_message>
<xml_diff>
--- a/TestData/Excel_Files/LoginCredentialDetails.xlsx
+++ b/TestData/Excel_Files/LoginCredentialDetails.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AWT Tester\eclipse-workspace\Awt_Project_Managment\TestData\Excel_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{955B28A6-D69B-45ED-AFE4-32C908FF5FA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8630A329-87DE-41DE-9189-BE3578D0D82E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2580" yWindow="2580" windowWidth="14400" windowHeight="7270" xr2:uid="{E28CADD0-9E9C-48D6-9692-C4E6C50E8CDC}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{E28CADD0-9E9C-48D6-9692-C4E6C50E8CDC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
   <si>
     <t>TestCaseId</t>
   </si>
@@ -58,64 +58,37 @@
     <t>OperatorScada#@2023</t>
   </si>
   <si>
-    <t>APMS-T132</t>
-  </si>
-  <si>
-    <t>APMS-T133</t>
-  </si>
-  <si>
-    <t>APMS-T134</t>
-  </si>
-  <si>
-    <t>APMS-T135</t>
-  </si>
-  <si>
-    <t>Tesla</t>
-  </si>
-  <si>
-    <t>APMS-T136</t>
-  </si>
-  <si>
-    <t>Tesla@123</t>
-  </si>
-  <si>
-    <t>Testing</t>
-  </si>
-  <si>
     <t>Testing@123</t>
   </si>
   <si>
-    <t>APMS-T143</t>
-  </si>
-  <si>
     <t>Email</t>
   </si>
   <si>
     <t>awtindia.sc@gmail.com</t>
   </si>
   <si>
-    <t>APMS-T144</t>
-  </si>
-  <si>
-    <t>nicoalastestla458@gmail.com</t>
-  </si>
-  <si>
-    <t>APMS-T153</t>
-  </si>
-  <si>
-    <t>Ankit@123</t>
-  </si>
-  <si>
-    <t>APMS-T154</t>
-  </si>
-  <si>
-    <t>AnkitYadav@1234</t>
-  </si>
-  <si>
-    <t>APMS-T155</t>
-  </si>
-  <si>
-    <t>AnkitYadav@12345$</t>
+    <t>SU-T721</t>
+  </si>
+  <si>
+    <t>superadminD</t>
+  </si>
+  <si>
+    <t>Rihand@123</t>
+  </si>
+  <si>
+    <t>SU-T722</t>
+  </si>
+  <si>
+    <t>SU-T723</t>
+  </si>
+  <si>
+    <t>SU-T730</t>
+  </si>
+  <si>
+    <t>SU-T731</t>
+  </si>
+  <si>
+    <t>niclosTesla@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -519,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8C46E38-2B1E-4402-BDC5-292DA50A6E9F}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -544,7 +517,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
@@ -560,106 +533,88 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>7</v>
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="B6" s="1"/>
       <c r="C6" s="4"/>
+      <c r="D6" s="4" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B7" s="1"/>
-      <c r="C7" s="4" t="s">
-        <v>16</v>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" t="s">
-        <v>21</v>
-      </c>
+      <c r="A8" s="1"/>
+      <c r="D8" s="4"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>23</v>
-      </c>
+      <c r="A9" s="1"/>
+      <c r="D9" s="4"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>25</v>
-      </c>
+      <c r="A10" s="2"/>
+      <c r="C10" s="4"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>27</v>
-      </c>
+      <c r="A11" s="1"/>
+      <c r="C11" s="4"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>29</v>
-      </c>
+      <c r="A12" s="1"/>
+      <c r="C12" s="4"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" s="1"/>
+      <c r="C13" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1" xr:uid="{4F447B3B-61D5-4B84-98CA-BB2FB17AF9C6}"/>
-    <hyperlink ref="C4" r:id="rId2" xr:uid="{44FA3455-F433-4672-8747-96EBABF495F1}"/>
-    <hyperlink ref="C5" r:id="rId3" xr:uid="{F70F74DB-E0ED-497D-A46A-A80DE8B48C29}"/>
-    <hyperlink ref="C7" r:id="rId4" xr:uid="{C0621982-136A-40A3-8716-B92ED6211AB7}"/>
-    <hyperlink ref="D9" r:id="rId5" xr:uid="{4E0708DC-BCB8-48B2-93AB-7B6268B178F0}"/>
-    <hyperlink ref="C10" r:id="rId6" xr:uid="{37D55B64-07BD-4510-9561-D5D4C639590C}"/>
-    <hyperlink ref="C11" r:id="rId7" xr:uid="{D988B4E8-12C5-482E-8303-D3DA0A78FBB9}"/>
-    <hyperlink ref="C12" r:id="rId8" xr:uid="{F434B21B-56F0-47FD-8CFC-7C51B5862AE5}"/>
+    <hyperlink ref="C4" r:id="rId1" xr:uid="{44FA3455-F433-4672-8747-96EBABF495F1}"/>
+    <hyperlink ref="C5" r:id="rId2" xr:uid="{F70F74DB-E0ED-497D-A46A-A80DE8B48C29}"/>
+    <hyperlink ref="D7" r:id="rId3" xr:uid="{A2DB13BB-FCDC-4395-B8F1-006EAF59B129}"/>
+    <hyperlink ref="D6" r:id="rId4" xr:uid="{ABEBC3DE-0B31-4C62-8A7E-75019DC1BF32}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Add View Village Test Cases
</commit_message>
<xml_diff>
--- a/TestData/Excel_Files/LoginCredentialDetails.xlsx
+++ b/TestData/Excel_Files/LoginCredentialDetails.xlsx
@@ -1,14 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AWT Tester\eclipse-workspace\Awt_Project_Managment\TestData\Excel_Files\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8630A329-87DE-41DE-9189-BE3578D0D82E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{CBFE821A-3478-4CDA-8606-82A942C4000E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{E28CADD0-9E9C-48D6-9692-C4E6C50E8CDC}"/>
   </bookViews>
@@ -17,6 +12,7 @@
     <sheet name="verifyLogInCredentialsTest" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -494,9 +490,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8C46E38-2B1E-4402-BDC5-292DA50A6E9F}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>

</xml_diff>